<commit_message>
with Sharp but maybe xuynya
</commit_message>
<xml_diff>
--- a/data2/mean_var.xlsx
+++ b/data2/mean_var.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.004791757064523466</v>
+        <v>0.004791757726395753</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000781303509927291</v>
+        <v>0.0007813039001524819</v>
       </c>
     </row>
     <row r="3">
@@ -470,36 +470,36 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0006086465917303407</v>
+        <v>0.000608646277943711</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0002040843815557264</v>
+        <v>0.0002040837046817845</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>GOOG</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0001695143254891404</v>
+        <v>0.0001578400726809109</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0001594834729978914</v>
+        <v>0.000157536931257989</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0001578396619367847</v>
+        <v>0.0001695143254891404</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001575370127499067</v>
+        <v>0.0001594834729978914</v>
       </c>
     </row>
     <row r="6">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0004710736249300026</v>
+        <v>0.0004710739231839039</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0003049394305589464</v>
+        <v>0.0003049396500722201</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0009251801536966433</v>
+        <v>0.0009251793916008272</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0003493146978488911</v>
+        <v>0.0003493147409145823</v>
       </c>
     </row>
     <row r="9">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5.970188140367831e-05</v>
+        <v>5.969832236319824e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001216726154668582</v>
+        <v>0.0001216729727845804</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.00104681465125513</v>
+        <v>0.001046814651255135</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0002793061297843101</v>
+        <v>0.0002793057785124484</v>
       </c>
     </row>
     <row r="12">
@@ -613,36 +613,36 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.001552509705759676</v>
+        <v>0.001552509833639477</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0003080523232319883</v>
+        <v>0.0003080525190485758</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AZN</t>
+          <t>PEP</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.0006208115044045069</v>
+        <v>0.0003452022700634803</v>
       </c>
       <c r="C15" t="n">
-        <v>0.000247212058372306</v>
+        <v>7.1983828376838e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PEP</t>
+          <t>AZN</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0003452033283062954</v>
+        <v>-0.0006208107451509798</v>
       </c>
       <c r="C16" t="n">
-        <v>7.198381845562408e-05</v>
+        <v>0.0002472116218947619</v>
       </c>
     </row>
     <row r="17">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0006712541210374818</v>
+        <v>0.0006712548222779616</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0001385908476279712</v>
+        <v>0.0001385912116243684</v>
       </c>
     </row>
     <row r="18">
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0006420888779063945</v>
+        <v>0.0006420875880178026</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0001811547783800865</v>
+        <v>0.0001811539506805654</v>
       </c>
     </row>
     <row r="20">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.00118796384579611</v>
+        <v>0.001187964627932078</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0003132064297257861</v>
+        <v>0.0003132064104617103</v>
       </c>
     </row>
     <row r="21">
@@ -704,36 +704,36 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.001280133347426345</v>
+        <v>0.001280131901946855</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0001753738572009153</v>
+        <v>0.0001753747607148026</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>INTU</t>
+          <t>AMGN</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.0008204260966541673</v>
+        <v>-0.0002138669875757005</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0001541022897302211</v>
+        <v>0.0002375851329806968</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AMGN</t>
+          <t>INTU</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.0002138662427210068</v>
+        <v>0.0008204261379338005</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0002375859822619504</v>
+        <v>0.0001541026309202054</v>
       </c>
     </row>
     <row r="24">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.002288413830975243</v>
+        <v>0.002288414744028531</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0003758883918143643</v>
+        <v>0.0003758874907965164</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.0009270748038564562</v>
+        <v>0.0009270755367825428</v>
       </c>
       <c r="C26" t="n">
-        <v>0.000114459557341981</v>
+        <v>0.0001144594514881142</v>
       </c>
     </row>
     <row r="27">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.0006499835544643284</v>
+        <v>0.0006499838885816938</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0003507270993650239</v>
+        <v>0.0003507276499620088</v>
       </c>
     </row>
     <row r="28">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0005934719437981652</v>
+        <v>0.0005934713532669781</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0001256384351955858</v>
+        <v>0.000125638818668137</v>
       </c>
     </row>
     <row r="29">
@@ -830,27 +830,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ADP</t>
+          <t>MU</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.0009929382738462311</v>
+        <v>0.001693402989727995</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0001108292658202764</v>
+        <v>0.001029879002263344</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>ADP</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.001693403530744327</v>
+        <v>0.000992937478419769</v>
       </c>
       <c r="C32" t="n">
-        <v>0.001029880303865003</v>
+        <v>0.0001108287177409622</v>
       </c>
     </row>
     <row r="33">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.001258297196007891</v>
+        <v>0.001258298230554382</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0002204923523310186</v>
+        <v>0.0002204926327720668</v>
       </c>
     </row>
     <row r="34">
@@ -886,62 +886,62 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.0001327458031665835</v>
+        <v>-0.0001327435953880019</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0001572050762375656</v>
+        <v>0.0001572055422603591</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>KLAC</t>
+          <t>LRCX</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0006617843299393226</v>
+        <v>0.001554779270507288</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0001763766165138962</v>
+        <v>0.0003175188223807012</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>LRCX</t>
+          <t>KLAC</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.001418680440532165</v>
+        <v>0.0006617849538736269</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0003013936562055045</v>
+        <v>0.000176377742102125</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GILD</t>
+          <t>MELI</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.001159193661535886</v>
+        <v>0.001414183280644268</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0002872737409330569</v>
+        <v>0.0005015673650968572</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MELI</t>
+          <t>GILD</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.001414183670894209</v>
+        <v>-0.001159193092263775</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0005015671580447068</v>
+        <v>0.0002872735440944644</v>
       </c>
     </row>
     <row r="40">
@@ -951,10 +951,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.0003879791839093986</v>
+        <v>0.0003879786706433413</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0002043002371787759</v>
+        <v>0.0002042997220563958</v>
       </c>
     </row>
     <row r="41">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.00011686133827663</v>
+        <v>0.0001168621770919631</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0002846231216477884</v>
+        <v>0.0002846239921258829</v>
       </c>
     </row>
     <row r="42">
@@ -977,36 +977,36 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.001123463416944211</v>
+        <v>0.001280820366687428</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0001482041413653911</v>
+        <v>0.0001526327418421319</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PYPL</t>
+          <t>SNPS</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0005074157314395192</v>
+        <v>0.001076807426562563</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0003085645244898223</v>
+        <v>0.0001280042808616382</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SNPS</t>
+          <t>PYPL</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.001076807426562563</v>
+        <v>0.0005074157314395192</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0001280042808616382</v>
+        <v>0.0003085645244898223</v>
       </c>
     </row>
     <row r="45">
@@ -1029,10 +1029,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.001000705800113524</v>
+        <v>0.001000704087030286</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0002465625177459078</v>
+        <v>0.0002465631699095578</v>
       </c>
     </row>
     <row r="47">
@@ -1055,62 +1055,62 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.001424262709251114</v>
+        <v>0.001424263413040009</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0002638559550257221</v>
+        <v>0.0002638560309284628</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MRVL</t>
+          <t>WDAY</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001894871996017122</v>
+        <v>-0.0006478477830791533</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0005145467722323421</v>
+        <v>0.0007386675435605258</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>WDAY</t>
+          <t>MRVL</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.0006478477830791533</v>
+        <v>0.001894871010761541</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0007386675435605258</v>
+        <v>0.0005145473683505556</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NXPI</t>
+          <t>FTNT</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.0005937391333899148</v>
+        <v>-1.452342082719582e-05</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0005494583205794864</v>
+        <v>0.0004721799121230202</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>FTNT</t>
+          <t>NXPI</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-1.452342082719582e-05</v>
+        <v>0.0005937381103851151</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0004721799121230202</v>
+        <v>0.0005494577051172493</v>
       </c>
     </row>
     <row r="53">
@@ -1133,10 +1133,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-4.714009009182164e-05</v>
+        <v>-4.713989730441069e-05</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0001640334026580059</v>
+        <v>0.0001640338333908919</v>
       </c>
     </row>
     <row r="55">
@@ -1146,10 +1146,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.001690815033646858</v>
+        <v>0.001690814103568938</v>
       </c>
       <c r="C55" t="n">
-        <v>0.0006042657338384508</v>
+        <v>0.0006042643448072175</v>
       </c>
     </row>
     <row r="56">
@@ -1159,23 +1159,23 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.001314376673720907</v>
+        <v>0.001314377003276264</v>
       </c>
       <c r="C56" t="n">
-        <v>0.000261005433103709</v>
+        <v>0.0002610052993351169</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>AEP</t>
+          <t>CPRT</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.0004447332685213867</v>
+        <v>0.001537434689359692</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0001255337589190014</v>
+        <v>0.000184575384017428</v>
       </c>
     </row>
     <row r="58">
@@ -1194,131 +1194,131 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CPRT</t>
+          <t>AEP</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.001537434689359692</v>
+        <v>0.0004447342210871816</v>
       </c>
       <c r="C59" t="n">
-        <v>0.000184575384017428</v>
+        <v>0.0001255333303717242</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>PAYX</t>
+          <t>MNST</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0007944872947181368</v>
+        <v>-0.0003253870869810081</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0001267025728627172</v>
+        <v>0.0002874577754103618</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>KDP</t>
+          <t>PAYX</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.486324691772094e-05</v>
+        <v>0.0007944879934807374</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0001231953909572918</v>
+        <v>0.0001267022309677935</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MNST</t>
+          <t>KDP</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>-0.0003253870869810081</v>
+        <v>2.486416858565427e-05</v>
       </c>
       <c r="C62" t="n">
-        <v>0.0002874577754103618</v>
+        <v>0.0001231958349491246</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>ROST</t>
+          <t>TEAM</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.0007842439428708786</v>
+        <v>-0.0005160409859583973</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0001762896724642949</v>
+        <v>0.0008129416636759335</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>TEAM</t>
+          <t>ROST</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.0005160409859583973</v>
+        <v>0.0007842419758300012</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0008129416636759335</v>
+        <v>0.0001762896607575369</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>KHC</t>
+          <t>FAST</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0008422566985826722</v>
+        <v>0.0007393852622347126</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0001654458669554324</v>
+        <v>0.000237101092428346</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MCHP</t>
+          <t>ODFL</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.001435790872162611</v>
+        <v>0.001530852491970737</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0002541682553790211</v>
+        <v>0.000284365347228002</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ODFL</t>
+          <t>KHC</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.001530852620385067</v>
+        <v>0.0008422548716767359</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0002843659447858218</v>
+        <v>0.0001654461098804011</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>FAST</t>
+          <t>MCHP</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.0007393845414575935</v>
+        <v>0.001435790485856591</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0002371016430728639</v>
+        <v>0.0002541671089951331</v>
       </c>
     </row>
     <row r="69">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.001099213610026367</v>
+        <v>0.001099212824391787</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0001990674293635316</v>
+        <v>0.0001990675577491658</v>
       </c>
     </row>
     <row r="70">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0002990654817915954</v>
+        <v>0.0002990666476850587</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0001148204025634927</v>
+        <v>0.0001148203702621627</v>
       </c>
     </row>
     <row r="72">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.0006981527272676755</v>
+        <v>0.0006981535920071758</v>
       </c>
       <c r="C72" t="n">
-        <v>0.0003375213286778599</v>
+        <v>0.0003375210087248839</v>
       </c>
     </row>
     <row r="73">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.000146592675702818</v>
+        <v>-0.0001465932538590275</v>
       </c>
       <c r="C73" t="n">
-        <v>0.0003799401571786591</v>
+        <v>0.0003799404094710131</v>
       </c>
     </row>
     <row r="74">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.001325893987408093</v>
+        <v>0.001325896358313684</v>
       </c>
       <c r="C74" t="n">
-        <v>0.0006030842399105992</v>
+        <v>0.0006030836269188352</v>
       </c>
     </row>
     <row r="75">
@@ -1406,36 +1406,36 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.0003398163994170235</v>
+        <v>-0.0003398158017141503</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0001958377582384927</v>
+        <v>0.0001958379840393211</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>XEL</t>
+          <t>LULU</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.0006535418478616922</v>
+        <v>0.0006031267234766266</v>
       </c>
       <c r="C76" t="n">
-        <v>0.000123123803756521</v>
+        <v>0.0004333103936674401</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LULU</t>
+          <t>XEL</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.0006031267234766266</v>
+        <v>0.0006535408186765775</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0004333103936674401</v>
+        <v>0.000123123541735914</v>
       </c>
     </row>
     <row r="78">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.001001692569308007</v>
+        <v>0.001001691522343329</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0002214382277020203</v>
+        <v>0.0002214376871376766</v>
       </c>
     </row>
     <row r="81">
@@ -1506,14 +1506,14 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>TTWO</t>
+          <t>SMCI</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.001459654289844646</v>
+        <v>0.0006797830151301731</v>
       </c>
       <c r="C83" t="n">
-        <v>0.0003452783591290246</v>
+        <v>0.001316613247760909</v>
       </c>
     </row>
     <row r="84">
@@ -1532,14 +1532,14 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>SMCI</t>
+          <t>TTWO</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0006797830151301731</v>
+        <v>0.001459654289844646</v>
       </c>
       <c r="C85" t="n">
-        <v>0.001316613247760909</v>
+        <v>0.0003452783591290246</v>
       </c>
     </row>
     <row r="86">

</xml_diff>

<commit_message>
add work with 10 and compare
</commit_message>
<xml_diff>
--- a/data2/mean_var.xlsx
+++ b/data2/mean_var.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.00479175694336796</v>
+        <v>0.004791757665818062</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0007813033556760727</v>
+        <v>0.0007813032928621058</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0006086454254940342</v>
+        <v>0.000608645605915446</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0002040837586865453</v>
+        <v>0.0002040837857321601</v>
       </c>
     </row>
     <row r="4">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0001695147100087647</v>
+        <v>0.0001695143254891404</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001594835865118768</v>
+        <v>0.0001594834729978914</v>
       </c>
     </row>
     <row r="6">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0004710736249300026</v>
+        <v>0.0004710736249300006</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0003049394305589464</v>
+        <v>0.0003049393018863124</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0009251801536966415</v>
+        <v>0.0009251791894286707</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0003493150197259198</v>
+        <v>0.0003493141629322204</v>
       </c>
     </row>
     <row r="9">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5.969831567204535e-05</v>
+        <v>5.969964529379418e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001216724881605824</v>
+        <v>0.0001216739966768324</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001046814358538758</v>
+        <v>0.001046814563293233</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0002793061552063483</v>
+        <v>0.0002793053719548725</v>
       </c>
     </row>
     <row r="12">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.001552510766624936</v>
+        <v>0.001552510498256412</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0003080523754253228</v>
+        <v>0.0003080523236351159</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0003452026008641008</v>
+        <v>0.0003452018075808366</v>
       </c>
       <c r="C15" t="n">
-        <v>7.198366818428937e-05</v>
+        <v>7.198372605589395e-05</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.0006208115044045144</v>
+        <v>-0.0006208114533140928</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0002472121835859683</v>
+        <v>0.0002472115920729881</v>
       </c>
     </row>
     <row r="17">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0006712561160274768</v>
+        <v>0.0006712556322502778</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0001385908352783491</v>
+        <v>0.0001385914332359263</v>
       </c>
     </row>
     <row r="18">
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0006420878540967865</v>
+        <v>0.0006420875316246322</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0001811538503930647</v>
+        <v>0.0001811537438775771</v>
       </c>
     </row>
     <row r="20">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.001187964236864084</v>
+        <v>0.001187964728761791</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0003132062073119949</v>
+        <v>0.0003132059667956394</v>
       </c>
     </row>
     <row r="21">
@@ -704,10 +704,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.001280133222899704</v>
+        <v>0.001280133834653497</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0001753738237623097</v>
+        <v>0.0001753743963529469</v>
       </c>
     </row>
     <row r="22">
@@ -717,10 +717,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.0002138664910059192</v>
+        <v>-0.0002138667392908129</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0002375846847024813</v>
+        <v>0.000237585266056228</v>
       </c>
     </row>
     <row r="23">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0008204280855021611</v>
+        <v>0.0008204271761229281</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0001541020240275119</v>
+        <v>0.0001541017881535345</v>
       </c>
     </row>
     <row r="24">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.002288414345067223</v>
+        <v>0.002288414088021248</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0003758881336930636</v>
+        <v>0.0003758880376423061</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.000927074998006717</v>
+        <v>0.000927075799857912</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0001144594227649211</v>
+        <v>0.0001144594749207517</v>
       </c>
     </row>
     <row r="27">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0005934716227477214</v>
+        <v>0.0005934731132288106</v>
       </c>
       <c r="C28" t="n">
-        <v>0.000125638491784172</v>
+        <v>0.0001256388937558624</v>
       </c>
     </row>
     <row r="29">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.00169340290655164</v>
+        <v>0.001693403530744332</v>
       </c>
       <c r="C31" t="n">
-        <v>0.001029880203536024</v>
+        <v>0.001029879590380019</v>
       </c>
     </row>
     <row r="32">
@@ -847,10 +847,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.0009929395162916108</v>
+        <v>0.0009929374784197721</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0001108287209766082</v>
+        <v>0.0001108286665838971</v>
       </c>
     </row>
     <row r="33">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.00125829719600789</v>
+        <v>0.001258296952996726</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0002204925230524289</v>
+        <v>0.0002204923429305079</v>
       </c>
     </row>
     <row r="34">
@@ -886,10 +886,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.0001327448599851579</v>
+        <v>-0.0001327448705179431</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0001572058171777389</v>
+        <v>0.0001572055698727408</v>
       </c>
     </row>
     <row r="36">
@@ -899,10 +899,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0006617829221084279</v>
+        <v>0.0006617827407904939</v>
       </c>
       <c r="C36" t="n">
-        <v>0.000176376088215248</v>
+        <v>0.0001763773517259716</v>
       </c>
     </row>
     <row r="37">
@@ -912,10 +912,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.001554779563702869</v>
+        <v>0.001566700094702903</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0003175193210789412</v>
+        <v>0.0003104625081012702</v>
       </c>
     </row>
     <row r="38">
@@ -925,10 +925,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.001414183280644267</v>
+        <v>0.001414183949166552</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0005015673941555149</v>
+        <v>0.0005015674530076113</v>
       </c>
     </row>
     <row r="39">
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.001159192807627741</v>
+        <v>-0.001159191387239844</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0002872736677585579</v>
+        <v>0.0002872738666978927</v>
       </c>
     </row>
     <row r="40">
@@ -951,10 +951,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.0003879782098750859</v>
+        <v>0.000387980598319661</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0002043001595252609</v>
+        <v>0.0002042996436444955</v>
       </c>
     </row>
     <row r="41">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.0001168588582013153</v>
+        <v>0.0001168592776088303</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0002846222666673385</v>
+        <v>0.000284622802170424</v>
       </c>
     </row>
     <row r="42">
@@ -977,10 +977,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.001123462986331379</v>
+        <v>0.00128081856973723</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0001482042936250954</v>
+        <v>0.0001526322847375969</v>
       </c>
     </row>
     <row r="43">
@@ -1029,10 +1029,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.001000704480189036</v>
+        <v>0.001000704873347741</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0002465623751987243</v>
+        <v>0.0002465634870941096</v>
       </c>
     </row>
     <row r="47">
@@ -1055,10 +1055,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.001424263061145577</v>
+        <v>0.001424261351124213</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0002638551557026518</v>
+        <v>0.0002638562768277243</v>
       </c>
     </row>
     <row r="49">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001894873062647172</v>
+        <v>0.001894873530529465</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0005145457210963086</v>
+        <v>0.000514546936844866</v>
       </c>
     </row>
     <row r="50">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.0005937376049807588</v>
+        <v>0.0005937377145825442</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0005494582061977875</v>
+        <v>0.0005494584153039738</v>
       </c>
     </row>
     <row r="53">
@@ -1133,10 +1133,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-4.713953727286663e-05</v>
+        <v>-4.713816668456906e-05</v>
       </c>
       <c r="C54" t="n">
-        <v>0.00016403351736342</v>
+        <v>0.0001640332605970512</v>
       </c>
     </row>
     <row r="55">
@@ -1146,10 +1146,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.00169081485626156</v>
+        <v>0.001690814678876192</v>
       </c>
       <c r="C55" t="n">
-        <v>0.000604266820927395</v>
+        <v>0.0006042654669548398</v>
       </c>
     </row>
     <row r="56">
@@ -1159,10 +1159,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.001314378569295074</v>
+        <v>0.001314377332831648</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0002610041822566004</v>
+        <v>0.0002610044563973783</v>
       </c>
     </row>
     <row r="57">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0004447362387138967</v>
+        <v>0.0004447341835887492</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0001255337754924465</v>
+        <v>0.0001255336465242655</v>
       </c>
     </row>
     <row r="59">
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.0007944876788206331</v>
+        <v>0.0007944876788206297</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0001267023311773661</v>
+        <v>0.0001267024294829454</v>
       </c>
     </row>
     <row r="62">
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2.486261892469078e-05</v>
+        <v>2.486386136307451e-05</v>
       </c>
       <c r="C62" t="n">
-        <v>0.0001231954653835451</v>
+        <v>0.0001231957457136036</v>
       </c>
     </row>
     <row r="63">
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.0007842420845790778</v>
+        <v>0.0007842429755685265</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0001762900285627821</v>
+        <v>0.0001762895872500151</v>
       </c>
     </row>
     <row r="65">
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0007393827821678647</v>
+        <v>0.0007393850219756604</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0002371016388306028</v>
+        <v>0.0002371015617992498</v>
       </c>
     </row>
     <row r="66">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.001530855069970332</v>
+        <v>0.001530851686953008</v>
       </c>
       <c r="C66" t="n">
-        <v>0.000284365456545301</v>
+        <v>0.0002843655950373925</v>
       </c>
     </row>
     <row r="67">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.000842256324641236</v>
+        <v>0.0008422560801025979</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0001654459502616318</v>
+        <v>0.0001654458931218229</v>
       </c>
     </row>
     <row r="68">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.001435790099550612</v>
+        <v>0.001435790602749374</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0002541677978398323</v>
+        <v>0.0002541677073462823</v>
       </c>
     </row>
     <row r="69">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.001099211779945579</v>
+        <v>0.001099213332814677</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0001990675472940608</v>
+        <v>0.0001990689199006978</v>
       </c>
     </row>
     <row r="70">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0002990654212003668</v>
+        <v>0.0002990670363161403</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0001148203180753507</v>
+        <v>0.0001148203081139296</v>
       </c>
     </row>
     <row r="72">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.0006981536675808673</v>
+        <v>0.0006981545323204765</v>
       </c>
       <c r="C72" t="n">
-        <v>0.0003375212445890138</v>
+        <v>0.0003375209144886727</v>
       </c>
     </row>
     <row r="73">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.000146591797633739</v>
+        <v>-0.0001465909195646053</v>
       </c>
       <c r="C73" t="n">
-        <v>0.0003799410873879154</v>
+        <v>0.0003799405498825283</v>
       </c>
     </row>
     <row r="74">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.001325893948998274</v>
+        <v>0.001325897103086899</v>
       </c>
       <c r="C74" t="n">
-        <v>0.0006030848188436064</v>
+        <v>0.0006030839141308234</v>
       </c>
     </row>
     <row r="75">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.0003398161005655759</v>
+        <v>-0.0003398160516988455</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0001958381274378446</v>
+        <v>0.0001958381130051867</v>
       </c>
     </row>
     <row r="76">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.0006535402619718986</v>
+        <v>0.0006535402619718953</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0001231239337072319</v>
+        <v>0.0001231231821603362</v>
       </c>
     </row>
     <row r="78">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.001001692569308013</v>
+        <v>0.001001692979017388</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0002214390720581215</v>
+        <v>0.0002214381520231295</v>
       </c>
     </row>
     <row r="81">

</xml_diff>